<commit_message>
ORFS 1.0.2  style change column order in Control_Inputs.xlsx  style update version number in ORFS_License.m  feat add date and time to the name of slprj folder and move it to Simulink_Cache folder  feat import signal from Control_Inputs.xlsx  refactor delete unnecessary scopes in Joystick.slx
</commit_message>
<xml_diff>
--- a/Control_Inputs.xlsx
+++ b/Control_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iwl/ORFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B235DD-750B-2841-8A38-CE10B28A6D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E6F9A1-D10E-3148-90CB-982164103B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16420" yWindow="3280" windowWidth="28260" windowHeight="17320" xr2:uid="{E3584A9E-F21B-3A46-B33D-B570640E8F6F}"/>
   </bookViews>
@@ -42,16 +42,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Throttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Elevator</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rudder</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Throttle</t>
   </si>
 </sst>
 </file>
@@ -77,7 +76,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -427,12 +426,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D76"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="19">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>